<commit_message>
Add AI recommendation feature to output page: implement AI 추천 산출물명 column with editing capability and automatic application to 산출물명 field
</commit_message>
<xml_diff>
--- a/service/datagather_service/학습 데이터셋.xlsx
+++ b/service/datagather_service/학습 데이터셋.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bitcamp\OneDrive\바탕 화면\LCA proj\AI service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdhg\Desktop\greensteel-main\service\datagather_service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B02A8DA-98A0-4528-A133-899DC5AA3C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2537D986-A770-41E0-A913-65D5B406876F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AC2A805E-2818-429D-9FBB-D042F27A31B6}"/>
+    <workbookView xWindow="2670" yWindow="2115" windowWidth="22065" windowHeight="10440" xr2:uid="{AC2A805E-2818-429D-9FBB-D042F27A31B6}"/>
   </bookViews>
   <sheets>
     <sheet name="학습 데이터 셋" sheetId="1" r:id="rId1"/>
@@ -18,26 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'학습 데이터 셋'!$A$1:$K$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="725">
   <si>
     <t>Label</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2229,13 +2220,16 @@
   <si>
     <t>액화 석유가스</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환ㅇ웣널</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2258,6 +2252,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF93C5FD"/>
+      <name val="__Inter_e8ce0c"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2273,7 +2273,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2296,6 +2296,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2305,7 +2314,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2323,6 +2332,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2642,17 +2654,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D64" workbookViewId="0">
+      <selection activeCell="M71" sqref="M71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="11" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2687,7 +2699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -2722,7 +2734,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -2755,7 +2767,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
@@ -2788,7 +2800,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -2821,7 +2833,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
         <v>104</v>
       </c>
@@ -2856,7 +2868,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2891,7 +2903,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -2926,7 +2938,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="33">
       <c r="A9" s="2" t="s">
         <v>55</v>
       </c>
@@ -2961,7 +2973,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -2996,7 +3008,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
@@ -3031,7 +3043,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -3064,7 +3076,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -3099,7 +3111,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
         <v>193</v>
       </c>
@@ -3134,7 +3146,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -3167,7 +3179,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -3200,7 +3212,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
         <v>271</v>
       </c>
@@ -3233,7 +3245,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11">
       <c r="A18" s="2" t="s">
         <v>281</v>
       </c>
@@ -3266,7 +3278,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -3299,7 +3311,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -3334,7 +3346,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3367,7 +3379,7 @@
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
@@ -3400,7 +3412,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
@@ -3433,7 +3445,7 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
         <v>713</v>
       </c>
@@ -3466,7 +3478,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
         <v>335</v>
       </c>
@@ -3499,7 +3511,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -3532,7 +3544,7 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11">
       <c r="A27" s="2" t="s">
         <v>354</v>
       </c>
@@ -3565,7 +3577,7 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
@@ -3598,7 +3610,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11">
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
@@ -3633,7 +3645,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11">
       <c r="A30" s="2" t="s">
         <v>18</v>
       </c>
@@ -3668,7 +3680,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11">
       <c r="A31" s="2" t="s">
         <v>723</v>
       </c>
@@ -3703,7 +3715,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
         <v>717</v>
       </c>
@@ -3738,7 +3750,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="33">
       <c r="A33" s="2" t="s">
         <v>718</v>
       </c>
@@ -3773,7 +3785,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11">
       <c r="A34" s="2" t="s">
         <v>407</v>
       </c>
@@ -3808,7 +3820,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11">
       <c r="A35" s="2" t="s">
         <v>26</v>
       </c>
@@ -3841,7 +3853,7 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11">
       <c r="A36" s="2" t="s">
         <v>427</v>
       </c>
@@ -3874,7 +3886,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11">
       <c r="A37" s="2" t="s">
         <v>444</v>
       </c>
@@ -3909,7 +3921,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11">
       <c r="A38" s="2" t="s">
         <v>50</v>
       </c>
@@ -3944,7 +3956,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11">
       <c r="A39" s="2" t="s">
         <v>257</v>
       </c>
@@ -3979,7 +3991,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11">
       <c r="A40" s="2" t="s">
         <v>257</v>
       </c>
@@ -4014,7 +4026,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11">
       <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
@@ -4049,7 +4061,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="33">
       <c r="A42" s="2" t="s">
         <v>11</v>
       </c>
@@ -4084,7 +4096,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11">
       <c r="A43" s="2" t="s">
         <v>22</v>
       </c>
@@ -4117,7 +4129,7 @@
       </c>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11">
       <c r="A44" s="2" t="s">
         <v>57</v>
       </c>
@@ -4152,7 +4164,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11">
       <c r="A45" s="2" t="s">
         <v>60</v>
       </c>
@@ -4187,7 +4199,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11">
       <c r="A46" s="2" t="s">
         <v>58</v>
       </c>
@@ -4222,7 +4234,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11">
       <c r="A47" s="2" t="s">
         <v>33</v>
       </c>
@@ -4255,7 +4267,7 @@
       </c>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11">
       <c r="A48" s="2" t="s">
         <v>31</v>
       </c>
@@ -4290,7 +4302,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11">
       <c r="A49" s="2" t="s">
         <v>551</v>
       </c>
@@ -4323,7 +4335,7 @@
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11">
       <c r="A50" s="2" t="s">
         <v>24</v>
       </c>
@@ -4356,7 +4368,7 @@
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11">
       <c r="A51" s="2" t="s">
         <v>37</v>
       </c>
@@ -4391,7 +4403,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="33">
       <c r="A52" s="2" t="s">
         <v>49</v>
       </c>
@@ -4426,7 +4438,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11">
       <c r="A53" s="2" t="s">
         <v>15</v>
       </c>
@@ -4459,7 +4471,7 @@
       </c>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11">
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
@@ -4494,7 +4506,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="33">
       <c r="A55" s="2" t="s">
         <v>601</v>
       </c>
@@ -4529,7 +4541,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11">
       <c r="A56" s="2" t="s">
         <v>713</v>
       </c>
@@ -4562,7 +4574,7 @@
       </c>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11">
       <c r="A57" s="2" t="s">
         <v>19</v>
       </c>
@@ -4597,7 +4609,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11">
       <c r="A58" s="2" t="s">
         <v>620</v>
       </c>
@@ -4632,7 +4644,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11">
       <c r="A59" s="2" t="s">
         <v>631</v>
       </c>
@@ -4667,7 +4679,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11">
       <c r="A60" s="2" t="s">
         <v>16</v>
       </c>
@@ -4702,7 +4714,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11">
       <c r="A61" s="2" t="s">
         <v>652</v>
       </c>
@@ -4735,7 +4747,7 @@
       </c>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11">
       <c r="A62" s="2" t="s">
         <v>213</v>
       </c>
@@ -4770,7 +4782,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11">
       <c r="A63" s="2" t="s">
         <v>48</v>
       </c>
@@ -4803,7 +4815,7 @@
       </c>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11">
       <c r="A64" s="2" t="s">
         <v>204</v>
       </c>
@@ -4836,7 +4848,7 @@
       </c>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11">
       <c r="A65" s="2" t="s">
         <v>204</v>
       </c>
@@ -4869,7 +4881,7 @@
       </c>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11">
       <c r="A66" s="2" t="s">
         <v>658</v>
       </c>
@@ -4902,7 +4914,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" s="5" customFormat="1" ht="18.75" thickBot="1">
       <c r="A67" s="3" t="s">
         <v>716</v>
       </c>
@@ -4933,9 +4945,11 @@
       <c r="J67" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="K67" s="3"/>
-    </row>
-    <row r="68" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K67" s="6" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="5" customFormat="1">
       <c r="A68" s="4" t="s">
         <v>719</v>
       </c>
@@ -4968,7 +4982,7 @@
       </c>
       <c r="K68" s="3"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11">
       <c r="A69" s="2" t="s">
         <v>27</v>
       </c>
@@ -5003,7 +5017,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11">
       <c r="A70" s="2" t="s">
         <v>29</v>
       </c>
@@ -5038,7 +5052,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="33">
       <c r="A71" s="2" t="s">
         <v>45</v>
       </c>
@@ -5071,7 +5085,7 @@
       </c>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11">
       <c r="A72" s="2" t="s">
         <v>46</v>
       </c>

</xml_diff>